<commit_message>
Move Ignored Errors to Own Class
In response to comments from @MarkBaker, implement ignoredError as a new class. This simplifies Cell by requiring only 1 new method, rather than 8+. This requires a slightly more complicated syntax.
```php
$cell->getIgnoredErrors()->setNumberScoredAsText(true);
```

Mark had also suggested that there might be a pre-existing regexp for processing the cells/cellranges when reading the sqref attribute. Those in Calculation are too complicated (read "non-performant") for this piece of code; the one in Coordinates is slightly less complicated than Calculation, but still more complicated than the one I'm using, and doesn't handle ranges.
</commit_message>
<xml_diff>
--- a/tests/data/Reader/XLSX/ignoreerror.xlsx
+++ b/tests/data/Reader/XLSX/ignoreerror.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CE407D2-EB62-4857-9236-B8C270E6B3BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25DE96DB-45BA-4D37-9FB1-500296D064AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{CF45F290-FCEF-40EF-A9F8-2B04BD427FDC}"/>
   </bookViews>
@@ -461,7 +461,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -731,15 +731,151 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9E5C2B3-6F51-4920-959B-4F76282BF58E}">
-  <dimension ref="A3"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <f>B1+1</f>
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <f>C1+2</f>
+        <v>4</v>
+      </c>
+      <c r="E1">
+        <f t="shared" ref="E1" si="0">D1+1</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <f t="shared" ref="C2:E2" si="1">B2+1</f>
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <f t="shared" ref="D2:D8" si="2">C2+2</f>
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:E3" si="3">B3+1</f>
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:E4" si="4">B4+1</f>
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:E5" si="5">B5+1</f>
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B6">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ref="C6:E6" si="6">B6+1</f>
+        <v>7</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B7">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <f t="shared" ref="C7:E7" si="7">B7+1</f>
+        <v>8</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="7"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ref="C8:E8" si="8">B8+1</f>
+        <v>9</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="8"/>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add FormulaRange to IgnoredErrors Possibilities
When I implemented IgnoredErrors (PR #3508), I dealt only with those that I understood well enough to come up with an example. I finally found an example for FormulaRange in the wild, so this PR adds it. Still unsupported are `calculatedColumn`, `emptyCellReferece`, `listDataValidation`, and `unlockedFormula`.
</commit_message>
<xml_diff>
--- a/tests/data/Reader/XLSX/ignoreerror.xlsx
+++ b/tests/data/Reader/XLSX/ignoreerror.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\formularange\tests\data\Reader\XLSX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25DE96DB-45BA-4D37-9FB1-500296D064AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{CF45F290-FCEF-40EF-A9F8-2B04BD427FDC}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="First" sheetId="2" r:id="rId1"/>
     <sheet name="Main" sheetId="1" r:id="rId2"/>
     <sheet name="Last" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -91,7 +90,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -437,7 +436,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1712149-EDD7-49A4-85FE-FA9A1413A1C1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -457,11 +456,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7E80E42-0455-4C7C-8C4F-1A23E0BE20C5}">
-  <dimension ref="A1:I12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -707,6 +706,12 @@
         <f>SQRT(-1)</f>
         <v>#NUM!</v>
       </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>4</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="str">
@@ -716,6 +721,30 @@
       <c r="C12" t="e">
         <f>LOG(0)</f>
         <v>#NUM!</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E13">
+        <v>3</v>
+      </c>
+      <c r="F13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E14">
+        <f>SUM(E11:E12)</f>
+        <v>3</v>
+      </c>
+      <c r="F14">
+        <f>SUM(F11:F12)</f>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -725,12 +754,13 @@
     <ignoredError sqref="D3 D5" formula="1"/>
     <ignoredError sqref="A12" twoDigitTextYear="1"/>
     <ignoredError sqref="C11" evalError="1"/>
+    <ignoredError sqref="F14" formulaRange="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9E5C2B3-6F51-4920-959B-4F76282BF58E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>